<commit_message>
Gives elec suppliers foresight of future RPS values in BAU
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BESHFoFRV/Boolean Elec Suppliers Have Foresight of Future RPS Values.xlsx
+++ b/InputData/ctrl-settings/BESHFoFRV/Boolean Elec Suppliers Have Foresight of Future RPS Values.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\ctrl-settings\BESHFoFRV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\ctrl-settings\BESHFoFRV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931CA74F-6D7E-4E04-8719-3F68AE8CEDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049D195-7A3D-49BF-A659-2474B28290D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31470" yWindow="2670" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BESHFoFRV" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -403,46 +416,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -460,21 +473,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Turn off RPS foresight
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BESHFoFRV/Boolean Elec Suppliers Have Foresight of Future RPS Values.xlsx
+++ b/InputData/ctrl-settings/BESHFoFRV/Boolean Elec Suppliers Have Foresight of Future RPS Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ctrl-settings\BESHFoFRV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC83E865-AC4C-42B7-94A5-3945F87A4DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3987D8DF-44E5-4C4D-96AD-E4F41610CCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>